<commit_message>
Scripting DPLKINV003-005 and DPLKINV003-010 until DPLKINV003-012
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV003-009 - Fixed Income - Upload Harga Pasar.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV003-009 - Fixed Income - Upload Harga Pasar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0A9F53-EBE3-46EB-B9F8-94ECF361AA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EC127F-8029-4484-AC20-EECF9BC7E862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>23</v>
       </c>
       <c r="G2" s="4">
-        <v>32382</v>
+        <v>47466</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>13</v>

</xml_diff>